<commit_message>
close #96: Add acronym check in `nome_simples` column
</commit_message>
<xml_diff>
--- a/input_data/data_errors_04/descricao.xlsx
+++ b/input_data/data_errors_04/descricao.xlsx
@@ -79,7 +79,7 @@
     <t xml:space="preserve">2.77</t>
   </si>
   <si>
-    <t xml:space="preserve">Seca</t>
+    <t xml:space="preserve">IDEB séries Finais</t>
   </si>
   <si>
     <t xml:space="preserve">Índice de risco de impacto para seca</t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">XX3</t>
   </si>
   <si>
-    <t xml:space="preserve">Vulnerabilidade</t>
+    <t xml:space="preserve">Vulnerabilidade Do IDEB</t>
   </si>
   <si>
     <t xml:space="preserve">Índice de vulnerabilidade</t>
@@ -423,10 +423,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.89"/>

</xml_diff>